<commit_message>
Simulation and efficiency update
</commit_message>
<xml_diff>
--- a/output/minutes_stats.xlsx
+++ b/output/minutes_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\05. Project\01. MUFC Performance 2021-2022\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855DC4F8-FF85-482D-8519-8F62373C6FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B750CD-2D2C-4A83-9939-D19F222F2D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>player</t>
   </si>
@@ -41,9 +41,24 @@
     <t>pl21_minutes</t>
   </si>
   <si>
+    <t>Daniel James</t>
+  </si>
+  <si>
     <t>Dean Henderson</t>
   </si>
   <si>
+    <t>Eric Bailly</t>
+  </si>
+  <si>
+    <t>Anthony Martial</t>
+  </si>
+  <si>
+    <t>Donny van de Beek</t>
+  </si>
+  <si>
+    <t>Juan Mata</t>
+  </si>
+  <si>
     <t>David de Gea</t>
   </si>
   <si>
@@ -59,15 +74,9 @@
     <t>Scott McTominay</t>
   </si>
   <si>
-    <t>Daniel James</t>
-  </si>
-  <si>
     <t>Victor LindelÃ¶f</t>
   </si>
   <si>
-    <t>Brandon Williams</t>
-  </si>
-  <si>
     <t>Fred</t>
   </si>
   <si>
@@ -105,24 +114,6 @@
   </si>
   <si>
     <t>Edinson Cavani</t>
-  </si>
-  <si>
-    <t>Axel Tuanzebe</t>
-  </si>
-  <si>
-    <t>Donny van de Beek</t>
-  </si>
-  <si>
-    <t>Jesse Lingard</t>
-  </si>
-  <si>
-    <t>Juan Mata</t>
-  </si>
-  <si>
-    <t>Eric Bailly</t>
-  </si>
-  <si>
-    <t>Anthony Martial</t>
   </si>
   <si>
     <t>max</t>
@@ -966,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -993,13 +984,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1125</v>
+        <v>910</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1125</v>
+        <v>910</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1007,13 +998,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2295</v>
+        <v>1125</v>
       </c>
       <c r="C3">
-        <v>3420</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3420</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1021,13 +1012,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3099</v>
+        <v>916</v>
       </c>
       <c r="C4">
-        <v>3111</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>3111</v>
+        <v>916</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1035,13 +1026,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3047</v>
+        <v>1480</v>
       </c>
       <c r="C5">
-        <v>2515</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>3047</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1049,13 +1040,13 @@
         <v>7</v>
       </c>
       <c r="B6">
+        <v>524</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>2456</v>
-      </c>
       <c r="D6">
-        <v>2456</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1063,13 +1054,13 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>2129</v>
+        <v>509</v>
       </c>
       <c r="C7">
-        <v>2387</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>2387</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,13 +1068,13 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>910</v>
+        <v>2295</v>
       </c>
       <c r="C8">
-        <v>2366</v>
+        <v>3420</v>
       </c>
       <c r="D8">
-        <v>2366</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1091,13 +1082,13 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>2585</v>
+        <v>3099</v>
       </c>
       <c r="C9">
-        <v>2355</v>
+        <v>3111</v>
       </c>
       <c r="D9">
-        <v>2585</v>
+        <v>3111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1105,13 +1096,13 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>188</v>
+        <v>3047</v>
       </c>
       <c r="C10">
-        <v>2120</v>
+        <v>2515</v>
       </c>
       <c r="D10">
-        <v>2120</v>
+        <v>3047</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1119,13 +1110,13 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>2390</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>2028</v>
+        <v>2456</v>
       </c>
       <c r="D11">
-        <v>2390</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1133,13 +1124,13 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>2129</v>
       </c>
       <c r="C12">
-        <v>1900</v>
+        <v>2387</v>
       </c>
       <c r="D12">
-        <v>1900</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1147,13 +1138,13 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2585</v>
       </c>
       <c r="C13">
-        <v>1831</v>
+        <v>2355</v>
       </c>
       <c r="D13">
-        <v>1831</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1161,13 +1152,13 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>2390</v>
       </c>
       <c r="C14">
-        <v>1801</v>
+        <v>2028</v>
       </c>
       <c r="D14">
-        <v>1801</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1175,13 +1166,13 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>3060</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1793</v>
+        <v>1900</v>
       </c>
       <c r="D15">
-        <v>3060</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1189,13 +1180,13 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>690</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1660</v>
+        <v>1831</v>
       </c>
       <c r="D16">
-        <v>1660</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1203,13 +1194,13 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>2654</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1601</v>
+        <v>1801</v>
       </c>
       <c r="D17">
-        <v>2654</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1217,13 +1208,13 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>1106</v>
+        <v>3060</v>
       </c>
       <c r="C18">
-        <v>1382</v>
+        <v>1793</v>
       </c>
       <c r="D18">
-        <v>1382</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1231,13 +1222,13 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>1897</v>
+        <v>690</v>
       </c>
       <c r="C19">
-        <v>1349</v>
+        <v>1660</v>
       </c>
       <c r="D19">
-        <v>1897</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1245,13 +1236,13 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>1822</v>
+        <v>2654</v>
       </c>
       <c r="C20">
-        <v>1271</v>
+        <v>1601</v>
       </c>
       <c r="D20">
-        <v>1822</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1259,13 +1250,13 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>2920</v>
+        <v>1106</v>
       </c>
       <c r="C21">
-        <v>1235</v>
+        <v>1382</v>
       </c>
       <c r="D21">
-        <v>2920</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1273,13 +1264,13 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>155</v>
+        <v>1897</v>
       </c>
       <c r="C22">
-        <v>1214</v>
+        <v>1349</v>
       </c>
       <c r="D22">
-        <v>1214</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1287,13 +1278,13 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>1375</v>
+        <v>1822</v>
       </c>
       <c r="C23">
-        <v>766</v>
+        <v>1271</v>
       </c>
       <c r="D23">
-        <v>1375</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1301,13 +1292,13 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>404</v>
+        <v>2920</v>
       </c>
       <c r="C24">
-        <v>508</v>
+        <v>1235</v>
       </c>
       <c r="D24">
-        <v>508</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1315,13 +1306,13 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>524</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>483</v>
+        <v>1214</v>
       </c>
       <c r="D25">
-        <v>524</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1329,83 +1320,13 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>1421</v>
+        <v>1375</v>
       </c>
       <c r="C26">
-        <v>367</v>
+        <v>766</v>
       </c>
       <c r="D26">
-        <v>1421</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27">
-        <v>509</v>
-      </c>
-      <c r="C27">
-        <v>235</v>
-      </c>
-      <c r="D27">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28">
-        <v>916</v>
-      </c>
-      <c r="C28">
-        <v>217</v>
-      </c>
-      <c r="D28">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29">
-        <v>1480</v>
-      </c>
-      <c r="C29">
-        <v>212</v>
-      </c>
-      <c r="D29">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30">
-        <v>910</v>
-      </c>
-      <c r="C30">
-        <v>126</v>
-      </c>
-      <c r="D30">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31">
-        <v>524</v>
-      </c>
-      <c r="C31">
-        <v>75</v>
-      </c>
-      <c r="D31">
-        <v>524</v>
+        <v>1375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>